<commit_message>
Adds improvements and changes
</commit_message>
<xml_diff>
--- a/dircab.xlsx
+++ b/dircab.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>Question
 order</t>
@@ -69,9 +69,6 @@
     <t>Est-ce que ton DGS t’a déjà posé la question : “en fait, ça consiste en quoi ton boulot” ?</t>
   </si>
   <si>
-    <t>Ton directeur des travaux s’est-il déjà plaint auprès du DGS parce que tu leur donnais trop de boulot et “franchement, à quoi ça sert de prévenir les riverains du blocage de leur rue pendant les travaux” ?</t>
-  </si>
-  <si>
     <t>As-tu déjà entendu cette phrase en pleine période électorale  “ Tu penses que le point et la rose c’est essentiel sur les bulletins de vote?”</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
   </si>
   <si>
     <t>Ton élu(e) a-t-il déjà exigé de parler après le Premier Ministre venu inaugurer une nouvelle école car « les gens, c’est moi qu’ils viennent voir et écouter » ?</t>
-  </si>
-  <si>
-    <t>T’a-t-on déjà demandé d’organiser la retransmission de la finale de la coupe d’Europe sur la place de la mairie la veille du match en te précisant : « on n’a pas de budget » ?</t>
   </si>
   <si>
     <t>Cost-killer</t>
@@ -172,7 +166,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -240,13 +234,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -279,6 +310,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -1375,7 +1415,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V761"/>
+  <dimension ref="A1:V760"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1994,13 +2034,9 @@
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
     </row>
-    <row r="22" ht="13.65" customHeight="1">
-      <c r="A22" s="9">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s" s="10">
-        <v>22</v>
-      </c>
+    <row r="22" ht="13.65" customHeight="1" hidden="1">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -2022,13 +2058,9 @@
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
     </row>
-    <row r="23" ht="13.65" customHeight="1">
-      <c r="A23" s="9">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s" s="10">
-        <v>23</v>
-      </c>
+    <row r="23" ht="13.65" customHeight="1" hidden="1">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -19714,53 +19746,29 @@
       <c r="U759" s="6"/>
       <c r="V759" s="6"/>
     </row>
-    <row r="760" ht="13.65" customHeight="1" hidden="1">
-      <c r="A760" s="6"/>
-      <c r="B760" s="6"/>
-      <c r="C760" s="6"/>
-      <c r="D760" s="6"/>
-      <c r="E760" s="6"/>
-      <c r="F760" s="6"/>
-      <c r="G760" s="6"/>
-      <c r="H760" s="6"/>
-      <c r="I760" s="6"/>
-      <c r="J760" s="6"/>
-      <c r="K760" s="6"/>
-      <c r="L760" s="6"/>
-      <c r="M760" s="6"/>
-      <c r="N760" s="6"/>
-      <c r="O760" s="6"/>
-      <c r="P760" s="6"/>
-      <c r="Q760" s="6"/>
-      <c r="R760" s="6"/>
-      <c r="S760" s="6"/>
-      <c r="T760" s="6"/>
-      <c r="U760" s="6"/>
-      <c r="V760" s="6"/>
-    </row>
-    <row r="761" ht="13.65" customHeight="1" hidden="1">
-      <c r="A761" s="6"/>
-      <c r="B761" s="6"/>
-      <c r="C761" s="6"/>
-      <c r="D761" s="6"/>
-      <c r="E761" s="6"/>
-      <c r="F761" s="6"/>
-      <c r="G761" s="6"/>
-      <c r="H761" s="6"/>
-      <c r="I761" s="6"/>
-      <c r="J761" s="6"/>
-      <c r="K761" s="6"/>
-      <c r="L761" s="6"/>
-      <c r="M761" s="6"/>
-      <c r="N761" s="6"/>
-      <c r="O761" s="6"/>
-      <c r="P761" s="6"/>
-      <c r="Q761" s="6"/>
-      <c r="R761" s="6"/>
-      <c r="S761" s="6"/>
-      <c r="T761" s="6"/>
-      <c r="U761" s="6"/>
-      <c r="V761" s="6"/>
+    <row r="760" ht="13.65" customHeight="1">
+      <c r="A760" s="11"/>
+      <c r="B760" s="12"/>
+      <c r="C760" s="12"/>
+      <c r="D760" s="12"/>
+      <c r="E760" s="12"/>
+      <c r="F760" s="12"/>
+      <c r="G760" s="12"/>
+      <c r="H760" s="12"/>
+      <c r="I760" s="12"/>
+      <c r="J760" s="12"/>
+      <c r="K760" s="12"/>
+      <c r="L760" s="12"/>
+      <c r="M760" s="12"/>
+      <c r="N760" s="12"/>
+      <c r="O760" s="12"/>
+      <c r="P760" s="12"/>
+      <c r="Q760" s="12"/>
+      <c r="R760" s="12"/>
+      <c r="S760" s="12"/>
+      <c r="T760" s="12"/>
+      <c r="U760" s="12"/>
+      <c r="V760" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -19782,107 +19790,107 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="23.1719" style="11" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="11" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="11" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="11" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="11" customWidth="1"/>
-    <col min="6" max="256" width="14.5" style="11" customWidth="1"/>
+    <col min="1" max="1" width="23.1719" style="14" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="14" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="14" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="14" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="14" customWidth="1"/>
+    <col min="6" max="256" width="14.5" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17" customHeight="1">
-      <c r="A1" t="s" s="12">
+      <c r="A1" t="s" s="15">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s" s="16">
+        <v>23</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" ht="17" customHeight="1">
+      <c r="A2" t="s" s="15">
         <v>24</v>
       </c>
-      <c r="B1" t="s" s="13">
+      <c r="B2" t="s" s="16">
         <v>25</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-    </row>
-    <row r="2" ht="17" customHeight="1">
-      <c r="A2" t="s" s="12">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" ht="17" customHeight="1">
+      <c r="A3" t="s" s="15">
         <v>26</v>
       </c>
-      <c r="B2" t="s" s="13">
+      <c r="B3" t="s" s="16">
         <v>27</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-    </row>
-    <row r="3" ht="17" customHeight="1">
-      <c r="A3" t="s" s="12">
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+    </row>
+    <row r="4" ht="17" customHeight="1">
+      <c r="A4" t="s" s="15">
         <v>28</v>
       </c>
-      <c r="B3" t="s" s="13">
+      <c r="B4" t="s" s="16">
         <v>29</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="4" ht="17" customHeight="1">
-      <c r="A4" t="s" s="12">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" ht="17" customHeight="1">
+      <c r="A5" t="s" s="15">
         <v>30</v>
       </c>
-      <c r="B4" t="s" s="13">
+      <c r="B5" t="s" s="16">
         <v>31</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-    </row>
-    <row r="5" ht="17" customHeight="1">
-      <c r="A5" t="s" s="12">
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" ht="17" customHeight="1">
+      <c r="A6" t="s" s="15">
         <v>32</v>
       </c>
-      <c r="B5" t="s" s="13">
+      <c r="B6" t="s" s="16">
         <v>33</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-    </row>
-    <row r="6" ht="17" customHeight="1">
-      <c r="A6" t="s" s="12">
-        <v>34</v>
-      </c>
-      <c r="B6" t="s" s="13">
-        <v>35</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
Adds new texts and deletes a few questions
</commit_message>
<xml_diff>
--- a/dircab.xlsx
+++ b/dircab.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>Question
 order</t>
@@ -21,64 +21,370 @@
     <t>Question</t>
   </si>
   <si>
-    <t>As-tu déjà eu la demande de ton maire d’écrire un mot manuscrit sur ses 8750 cartes de vœux parce que “envoyer une carte sans mot manuscrit, ça ne sert à rien” ?</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Est-ce que ton DGS t’a déjà posé la question : « </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>En fait, ça consiste en quoi ton boulot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> » ?</t>
+    </r>
   </si>
   <si>
-    <t>T’est-il déjà arrivé de nourrir le chat de ton élu pendant ses vacances, parce que “tu n’as que ça à faire quand je suis absent” ?</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">T’est-il déjà arrivé de nourrir le chat de ton élu(e) pendant ses vacances, parce qu’il (elle) pense : </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>« Tu n’as que ça à faire quand je suis absent(e)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> » ?</t>
+    </r>
   </si>
   <si>
-    <t>As-tu réécrit le discours de ton élu pour la cérémonie du 8 mai le 7 mai à 20h30, parce que franchement, “le copié/collé de celui de l’année dernière, ça ne va pas” ?</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Un riverain t’a-t-il demandé de couper trois arbres du trottoir face à son domicile : « </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Parce que l’été,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>on a de l’ombre dans le jardin, c’est intolérable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> » ?</t>
+    </r>
   </si>
   <si>
-    <t>Ton élu t’a-t-il déjà demandé de le représenter à l’AG du club de ping pong le samedi soir du weekend de l’ascension, parce qu’il a une réunion très importante dont il ne peut pas te parler, “c’est politique” ?</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>T’est-il arrivé d’organiser le mariage de ton élu(e), pour ces deux raisons : « </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>C’est hautement politique et je n’ai confiance qu’en toi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> » ?</t>
+    </r>
   </si>
   <si>
-    <t>T’est-il arrivé d’organiser le mariage de ton élu, parce que “c’est hautement politique et je n’ai confiance qu’en toi” ?</t>
+    <t>Ton élu(e) t’a-t-il (elle) déjà demandé : « Tu arrives à avoir une vie privée, toi ? Parce que moi, non » ?</t>
   </si>
   <si>
-    <t>Es-tu déjà allé annoncer à l’adjointe à la culture que ton maire lui retire sa délégation, parce que pour lui “vraiment, c’est une bonne copine, je n’ai pas le coeur de le faire” ?</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Est-ce que ton élu(e) t’a demandé ce que tu pensais de distribuer des roses à toutes les femmes qui bossent dans ta collectivité parce que quand même, “</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>il faut bien marquer le coup et donner du sens au 8 mars</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>” ?</t>
+    </r>
   </si>
   <si>
-    <t>As-tu annoncé au groupe EELV que le plan climat de la ville serait voté au prochain mandat, parce que, pour ton maire “ça leur apprendra à présenter un candidat aux cantonales contre moi” ?</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>L’association “Mieux vivre son quartier” t’a-t-elle déjà réclamé une subvention de 50 000 euros dans le cadre d’un déplacement éco-humaniste solidaire à New York car “</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>c’est super-important d’ouvrir nos esprits vers d’autres cultures</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>” ?</t>
+    </r>
   </si>
   <si>
-    <t>Ton élu t’a-t-il déjà demandé si tu pensais qu’il pourrait devenir ministre, parce que “honnêtement, à part moi, je ne vois personne” ?</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Ton DGS t’a-t-il déjà demandé si ta présence à ses réunions avec le maire est utile car il pense : «</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> Vraiment, tu as d’autres choses à faire</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> » ?</t>
+    </r>
   </si>
   <si>
-    <t>Ton élu t’a-t-il déjà demandé “tu arrives à avoir une vie privée, toi ? parce que moi, non” ?</t>
+    <t>As-tu déjà entendu cette phrase en pleine période électorale : « Tu penses que le poing et la rose c’est essentiel sur les bulletins de vote » ?</t>
   </si>
   <si>
-    <t>Est-ce que ton élu t’a demandé ce que tu pensais de distribuer des roses à toutes les femmes qui bossent dans ta collectivité parce quand même, “il faut bien marquer le coup et donner du sens au 8 mars” ?</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Ton intérêt pour les finances de la ville a-t-il déjà provoqué l’étonnement de ton DGS car “</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>le budget, ce n’est pas politique</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>” ?</t>
+    </r>
   </si>
   <si>
-    <t>L’association “mieux vivre son quartier” t’a-t-elle déjà réclamé une subvention de 50 000 euros dans le cadre d’un déplacement éco-humanisme solidaire à New York car “c’est super important d’ouvrir nos esprits vers d’autres cultures” ?</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>As-tu réécrit le discours de ton élu(e) pour la cérémonie du 8-Mai le 7 mai à 20 h 30, parce que franchement, “</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>le copié/collé de celui de l’année dernière, ça ne va pas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>” ?</t>
+    </r>
   </si>
   <si>
-    <t>Un riverain t’a-t-il demandé de couper 3 arbres du trottoir face à leur domicile parce que l’été, “on a que de l’ombre dans le jardin, c’est intolérable” ?</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>As-tu déjà eu la demande de ton maire d’écrire un mot manuscrit sur ses 8 750 cartes de vœux parce que “</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>envoyer une carte sans mot manuscrit, ça ne sert à rien</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>” ?</t>
+    </r>
   </si>
   <si>
-    <t>As-tu jamais reçu un administré pour qu’il te fasse une ristourne sur ses impôts locaux, parce que “je n’ai pas d’enfant, donc, je ne vois pas pourquoi je financerais les repas des cantines” ?</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Es-tu déjà allé(e)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>annoncer à l’adjointe à la Culture que ton maire lui retire sa délégation, parce que pour lui : «</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> Vraiment, c’est une bonne copine, je n’ai pas le cœur de le faire</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> » ?</t>
+    </r>
   </si>
   <si>
-    <t>Ton DGS t’a-t-il déjà demandé si ta présence à ses réunions avec le Maire est utile car “vraiment, tu as d’autres choses à faire” ?</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Ton élu(e) a-t-il (elle) déjà exigé de parler après le Premier ministre venu inaugurer une nouvelle école car il (elle) pense : « </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Les gens, c’est moi qu’ils viennent voir et écouter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> » ?</t>
+    </r>
   </si>
   <si>
-    <t>Ton intérêt pour les finances de la ville a-t-il déjà provoqué l’étonnement de ton DGS car “ le budget, ce n’est pas politique” ?</t>
-  </si>
-  <si>
-    <t>Est-ce que ton DGS t’a déjà posé la question : “en fait, ça consiste en quoi ton boulot” ?</t>
-  </si>
-  <si>
-    <t>As-tu déjà entendu cette phrase en pleine période électorale  “ Tu penses que le point et la rose c’est essentiel sur les bulletins de vote?”</t>
-  </si>
-  <si>
-    <t>As-tu déjà été envoyé(e) comme émissaire auprès du groupe PC pour leur annoncer que le Modem intégrait la majorité parce que : « finalement, il n’y a pas de grande différence entre nous, regarde, ils ont voté le passage au menu bio pour les cantines » ?</t>
-  </si>
-  <si>
-    <t>T’es-tu déjà retrouvé(e) en réunion avec 3 associations différentes à qui ton adjoint(e) au sport a octroyé le même créneau horaire pour l’utilisation du gymnase avec comme seule solution de sa part « ben les scolaires, tu me les cales le dimanche matin, les seniors le mercredi à 21h et le badminton tu les déplaces sur le terrain découvert » ?</t>
-  </si>
-  <si>
-    <t>Ton élu(e) a-t-il déjà exigé de parler après le Premier Ministre venu inaugurer une nouvelle école car « les gens, c’est moi qu’ils viennent voir et écouter » ?</t>
+    <t>Ton élu(e) t’a-t-il (elle) déjà demandé de le représenter à l’AG du club de ping-pong le samedi soir du week-end de l’Ascension, parce que sa présence est requise pour une réunion “hautement confidentielle et politique”.</t>
   </si>
   <si>
     <t>Cost-killer</t>
@@ -124,7 +430,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -144,6 +450,17 @@
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i val="1"/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="11"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -323,7 +640,7 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -351,6 +668,7 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffff0000"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1415,7 +1733,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V760"/>
+  <dimension ref="A1:V755"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1894,13 +2212,9 @@
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
     </row>
-    <row r="17" ht="13.65" customHeight="1">
-      <c r="A17" s="9">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s" s="10">
-        <v>17</v>
-      </c>
+    <row r="17" ht="13.65" customHeight="1" hidden="1">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1922,13 +2236,9 @@
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
     </row>
-    <row r="18" ht="13.65" customHeight="1">
-      <c r="A18" s="9">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s" s="10">
-        <v>18</v>
-      </c>
+    <row r="18" ht="13.65" customHeight="1" hidden="1">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1950,13 +2260,9 @@
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
     </row>
-    <row r="19" ht="13.65" customHeight="1">
-      <c r="A19" s="9">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s" s="10">
-        <v>19</v>
-      </c>
+    <row r="19" ht="13.65" customHeight="1" hidden="1">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -1978,13 +2284,9 @@
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
     </row>
-    <row r="20" ht="13.65" customHeight="1">
-      <c r="A20" s="9">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s" s="10">
-        <v>20</v>
-      </c>
+    <row r="20" ht="13.65" customHeight="1" hidden="1">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -2006,13 +2308,9 @@
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
     </row>
-    <row r="21" ht="13.65" customHeight="1">
-      <c r="A21" s="9">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s" s="10">
-        <v>21</v>
-      </c>
+    <row r="21" ht="13.65" customHeight="1" hidden="1">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -19626,149 +19924,29 @@
       <c r="U754" s="6"/>
       <c r="V754" s="6"/>
     </row>
-    <row r="755" ht="13.65" customHeight="1" hidden="1">
-      <c r="A755" s="6"/>
-      <c r="B755" s="6"/>
-      <c r="C755" s="6"/>
-      <c r="D755" s="6"/>
-      <c r="E755" s="6"/>
-      <c r="F755" s="6"/>
-      <c r="G755" s="6"/>
-      <c r="H755" s="6"/>
-      <c r="I755" s="6"/>
-      <c r="J755" s="6"/>
-      <c r="K755" s="6"/>
-      <c r="L755" s="6"/>
-      <c r="M755" s="6"/>
-      <c r="N755" s="6"/>
-      <c r="O755" s="6"/>
-      <c r="P755" s="6"/>
-      <c r="Q755" s="6"/>
-      <c r="R755" s="6"/>
-      <c r="S755" s="6"/>
-      <c r="T755" s="6"/>
-      <c r="U755" s="6"/>
-      <c r="V755" s="6"/>
-    </row>
-    <row r="756" ht="13.65" customHeight="1" hidden="1">
-      <c r="A756" s="6"/>
-      <c r="B756" s="6"/>
-      <c r="C756" s="6"/>
-      <c r="D756" s="6"/>
-      <c r="E756" s="6"/>
-      <c r="F756" s="6"/>
-      <c r="G756" s="6"/>
-      <c r="H756" s="6"/>
-      <c r="I756" s="6"/>
-      <c r="J756" s="6"/>
-      <c r="K756" s="6"/>
-      <c r="L756" s="6"/>
-      <c r="M756" s="6"/>
-      <c r="N756" s="6"/>
-      <c r="O756" s="6"/>
-      <c r="P756" s="6"/>
-      <c r="Q756" s="6"/>
-      <c r="R756" s="6"/>
-      <c r="S756" s="6"/>
-      <c r="T756" s="6"/>
-      <c r="U756" s="6"/>
-      <c r="V756" s="6"/>
-    </row>
-    <row r="757" ht="13.65" customHeight="1" hidden="1">
-      <c r="A757" s="6"/>
-      <c r="B757" s="6"/>
-      <c r="C757" s="6"/>
-      <c r="D757" s="6"/>
-      <c r="E757" s="6"/>
-      <c r="F757" s="6"/>
-      <c r="G757" s="6"/>
-      <c r="H757" s="6"/>
-      <c r="I757" s="6"/>
-      <c r="J757" s="6"/>
-      <c r="K757" s="6"/>
-      <c r="L757" s="6"/>
-      <c r="M757" s="6"/>
-      <c r="N757" s="6"/>
-      <c r="O757" s="6"/>
-      <c r="P757" s="6"/>
-      <c r="Q757" s="6"/>
-      <c r="R757" s="6"/>
-      <c r="S757" s="6"/>
-      <c r="T757" s="6"/>
-      <c r="U757" s="6"/>
-      <c r="V757" s="6"/>
-    </row>
-    <row r="758" ht="13.65" customHeight="1" hidden="1">
-      <c r="A758" s="6"/>
-      <c r="B758" s="6"/>
-      <c r="C758" s="6"/>
-      <c r="D758" s="6"/>
-      <c r="E758" s="6"/>
-      <c r="F758" s="6"/>
-      <c r="G758" s="6"/>
-      <c r="H758" s="6"/>
-      <c r="I758" s="6"/>
-      <c r="J758" s="6"/>
-      <c r="K758" s="6"/>
-      <c r="L758" s="6"/>
-      <c r="M758" s="6"/>
-      <c r="N758" s="6"/>
-      <c r="O758" s="6"/>
-      <c r="P758" s="6"/>
-      <c r="Q758" s="6"/>
-      <c r="R758" s="6"/>
-      <c r="S758" s="6"/>
-      <c r="T758" s="6"/>
-      <c r="U758" s="6"/>
-      <c r="V758" s="6"/>
-    </row>
-    <row r="759" ht="13.65" customHeight="1" hidden="1">
-      <c r="A759" s="6"/>
-      <c r="B759" s="6"/>
-      <c r="C759" s="6"/>
-      <c r="D759" s="6"/>
-      <c r="E759" s="6"/>
-      <c r="F759" s="6"/>
-      <c r="G759" s="6"/>
-      <c r="H759" s="6"/>
-      <c r="I759" s="6"/>
-      <c r="J759" s="6"/>
-      <c r="K759" s="6"/>
-      <c r="L759" s="6"/>
-      <c r="M759" s="6"/>
-      <c r="N759" s="6"/>
-      <c r="O759" s="6"/>
-      <c r="P759" s="6"/>
-      <c r="Q759" s="6"/>
-      <c r="R759" s="6"/>
-      <c r="S759" s="6"/>
-      <c r="T759" s="6"/>
-      <c r="U759" s="6"/>
-      <c r="V759" s="6"/>
-    </row>
-    <row r="760" ht="13.65" customHeight="1">
-      <c r="A760" s="11"/>
-      <c r="B760" s="12"/>
-      <c r="C760" s="12"/>
-      <c r="D760" s="12"/>
-      <c r="E760" s="12"/>
-      <c r="F760" s="12"/>
-      <c r="G760" s="12"/>
-      <c r="H760" s="12"/>
-      <c r="I760" s="12"/>
-      <c r="J760" s="12"/>
-      <c r="K760" s="12"/>
-      <c r="L760" s="12"/>
-      <c r="M760" s="12"/>
-      <c r="N760" s="12"/>
-      <c r="O760" s="12"/>
-      <c r="P760" s="12"/>
-      <c r="Q760" s="12"/>
-      <c r="R760" s="12"/>
-      <c r="S760" s="12"/>
-      <c r="T760" s="12"/>
-      <c r="U760" s="12"/>
-      <c r="V760" s="13"/>
+    <row r="755" ht="13.65" customHeight="1">
+      <c r="A755" s="11"/>
+      <c r="B755" s="12"/>
+      <c r="C755" s="12"/>
+      <c r="D755" s="12"/>
+      <c r="E755" s="12"/>
+      <c r="F755" s="12"/>
+      <c r="G755" s="12"/>
+      <c r="H755" s="12"/>
+      <c r="I755" s="12"/>
+      <c r="J755" s="12"/>
+      <c r="K755" s="12"/>
+      <c r="L755" s="12"/>
+      <c r="M755" s="12"/>
+      <c r="N755" s="12"/>
+      <c r="O755" s="12"/>
+      <c r="P755" s="12"/>
+      <c r="Q755" s="12"/>
+      <c r="R755" s="12"/>
+      <c r="S755" s="12"/>
+      <c r="T755" s="12"/>
+      <c r="U755" s="12"/>
+      <c r="V755" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -19800,10 +19978,10 @@
   <sheetData>
     <row r="1" ht="17" customHeight="1">
       <c r="A1" t="s" s="15">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s" s="16">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
@@ -19811,10 +19989,10 @@
     </row>
     <row r="2" ht="17" customHeight="1">
       <c r="A2" t="s" s="15">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s" s="16">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
@@ -19822,10 +20000,10 @@
     </row>
     <row r="3" ht="17" customHeight="1">
       <c r="A3" t="s" s="15">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s" s="16">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -19833,10 +20011,10 @@
     </row>
     <row r="4" ht="17" customHeight="1">
       <c r="A4" t="s" s="15">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s" s="16">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
@@ -19844,10 +20022,10 @@
     </row>
     <row r="5" ht="17" customHeight="1">
       <c r="A5" t="s" s="15">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s" s="16">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
@@ -19855,10 +20033,10 @@
     </row>
     <row r="6" ht="17" customHeight="1">
       <c r="A6" t="s" s="15">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s" s="16">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>

</xml_diff>

<commit_message>
Fixes the shuffling and changes copy
</commit_message>
<xml_diff>
--- a/dircab.xlsx
+++ b/dircab.xlsx
@@ -27,7 +27,7 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>Est-ce que ton DGS t’a déjà posé la question : « </t>
+      <t>Est-ce que ton DGS t’a déjà posé la question : &lt;em&gt;« </t>
     </r>
     <r>
       <rPr>
@@ -44,7 +44,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t> » ?</t>
+      <t> »</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;/em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> ?</t>
     </r>
   </si>
   <si>
@@ -55,6 +71,14 @@
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">T’est-il déjà arrivé de nourrir le chat de ton élu(e) pendant ses vacances, parce qu’il (elle) pense : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;em&gt;</t>
     </r>
     <r>
       <rPr>
@@ -71,7 +95,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t> » ?</t>
+      <t> »</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;/em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> ?</t>
     </r>
   </si>
   <si>
@@ -81,7 +121,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>Un riverain t’a-t-il demandé de couper trois arbres du trottoir face à son domicile : « </t>
+      <t xml:space="preserve">Un riverain t’a-t-il demandé de couper trois arbres du trottoir face à son domicile : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>« </t>
     </r>
     <r>
       <rPr>
@@ -115,7 +171,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t> » ?</t>
+      <t> »</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;/em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> ?</t>
     </r>
   </si>
   <si>
@@ -125,7 +197,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>T’est-il arrivé d’organiser le mariage de ton élu(e), pour ces deux raisons : « </t>
+      <t xml:space="preserve">T’est-il arrivé d’organiser le mariage de ton élu(e), pour ces deux raisons : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>« </t>
     </r>
     <r>
       <rPr>
@@ -142,11 +230,27 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t> » ?</t>
+      <t> »</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;/em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> ?</t>
     </r>
   </si>
   <si>
-    <t>Ton élu(e) t’a-t-il (elle) déjà demandé : « Tu arrives à avoir une vie privée, toi ? Parce que moi, non » ?</t>
+    <t>Ton élu(e) t’a-t-il (elle) déjà demandé : &lt;em&gt;« Tu arrives à avoir une vie privée, toi ? Parce que moi, non »&lt;/em&gt; ?</t>
   </si>
   <si>
     <r>
@@ -155,7 +259,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>Est-ce que ton élu(e) t’a demandé ce que tu pensais de distribuer des roses à toutes les femmes qui bossent dans ta collectivité parce que quand même, “</t>
+      <t xml:space="preserve">Est-ce que ton élu(e) t’a demandé ce que tu pensais de distribuer des roses à toutes les femmes qui bossent dans ta collectivité parce que quand même, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>“</t>
     </r>
     <r>
       <rPr>
@@ -172,7 +292,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>” ?</t>
+      <t>”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;/em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> ?</t>
     </r>
   </si>
   <si>
@@ -182,7 +318,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>L’association “Mieux vivre son quartier” t’a-t-elle déjà réclamé une subvention de 50 000 euros dans le cadre d’un déplacement éco-humaniste solidaire à New York car “</t>
+      <t xml:space="preserve">L’association “Mieux vivre son quartier” t’a-t-elle déjà réclamé une subvention de 50 000 euros dans le cadre d’un déplacement éco-humaniste solidaire à New York car </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>“</t>
     </r>
     <r>
       <rPr>
@@ -199,7 +351,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>” ?</t>
+      <t>”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;/em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> ?</t>
     </r>
   </si>
   <si>
@@ -209,7 +377,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>Ton DGS t’a-t-il déjà demandé si ta présence à ses réunions avec le maire est utile car il pense : «</t>
+      <t xml:space="preserve">Ton DGS t’a-t-il déjà demandé si ta présence à ses réunions avec le maire est utile car il pense : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>«</t>
     </r>
     <r>
       <rPr>
@@ -226,11 +410,27 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t> » ?</t>
+      <t> »</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;/em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> ?</t>
     </r>
   </si>
   <si>
-    <t>As-tu déjà entendu cette phrase en pleine période électorale : « Tu penses que le poing et la rose c’est essentiel sur les bulletins de vote » ?</t>
+    <t>As-tu déjà entendu cette phrase en pleine période électorale : &lt;em&gt;« Tu penses que le poing et la rose c’est essentiel sur les bulletins de vote »&lt;/em&gt; ?</t>
   </si>
   <si>
     <r>
@@ -239,7 +439,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>Ton intérêt pour les finances de la ville a-t-il déjà provoqué l’étonnement de ton DGS car “</t>
+      <t xml:space="preserve">Ton intérêt pour les finances de la ville a-t-il déjà provoqué l’étonnement de ton DGS car </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>“</t>
     </r>
     <r>
       <rPr>
@@ -256,7 +472,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>” ?</t>
+      <t>”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;/em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> ?</t>
     </r>
   </si>
   <si>
@@ -266,7 +498,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>As-tu réécrit le discours de ton élu(e) pour la cérémonie du 8-Mai le 7 mai à 20 h 30, parce que franchement, “</t>
+      <t xml:space="preserve">As-tu réécrit le discours de ton élu(e) pour la cérémonie du 8-Mai le 7 mai à 20 h 30, parce que franchement, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>“</t>
     </r>
     <r>
       <rPr>
@@ -283,7 +531,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>” ?</t>
+      <t>”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;/em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> ?</t>
     </r>
   </si>
   <si>
@@ -293,7 +557,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>As-tu déjà eu la demande de ton maire d’écrire un mot manuscrit sur ses 8 750 cartes de vœux parce que “</t>
+      <t xml:space="preserve">As-tu déjà eu la demande de ton maire d’écrire un mot manuscrit sur ses 8 750 cartes de vœux parce que </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>“</t>
     </r>
     <r>
       <rPr>
@@ -310,7 +590,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>” ?</t>
+      <t>”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;/em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> ?</t>
     </r>
   </si>
   <si>
@@ -336,7 +632,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>annoncer à l’adjointe à la Culture que ton maire lui retire sa délégation, parce que pour lui : «</t>
+      <t xml:space="preserve">annoncer à l’adjointe à la Culture que ton maire lui retire sa délégation, parce que pour lui : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>«</t>
     </r>
     <r>
       <rPr>
@@ -353,7 +665,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t> » ?</t>
+      <t> »</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;/em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> ?</t>
     </r>
   </si>
   <si>
@@ -363,7 +691,23 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>Ton élu(e) a-t-il (elle) déjà exigé de parler après le Premier ministre venu inaugurer une nouvelle école car il (elle) pense : « </t>
+      <t xml:space="preserve">Ton élu(e) a-t-il (elle) déjà exigé de parler après le Premier ministre venu inaugurer une nouvelle école car il (elle) pense : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>« </t>
     </r>
     <r>
       <rPr>
@@ -380,11 +724,27 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t> » ?</t>
+      <t> »</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;/em&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> ?</t>
     </r>
   </si>
   <si>
-    <t>Ton élu(e) t’a-t-il (elle) déjà demandé de le représenter à l’AG du club de ping-pong le samedi soir du week-end de l’Ascension, parce que sa présence est requise pour une réunion “hautement confidentielle et politique”.</t>
+    <t>Ton élu(e) t’a-t-il (elle) déjà demandé de le représenter à l’AG du club de ping-pong le samedi soir du week-end de l’Ascension, parce que sa présence est requise pour une réunion &lt;em&gt;“hautement confidentielle et politique”&lt;/em&gt;.</t>
   </si>
   <si>
     <t>Cost-killer</t>

</xml_diff>